<commit_message>
Cambio de implementacion hamilton comunidad
</commit_message>
<xml_diff>
--- a/Analisis de Cantidad de Vertices.xlsx
+++ b/Analisis de Cantidad de Vertices.xlsx
@@ -1,31 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan29reyes/Desktop/analisis_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901DF28D-A8BC-1543-831C-FCE514D95362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5082FC0A-8265-EA41-9CBF-EFA124CC4D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{36B05C6E-00E7-8741-8E22-DAB7CBFD8F63}"/>
+    <workbookView xWindow="-20" yWindow="620" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{36B05C6E-00E7-8741-8E22-DAB7CBFD8F63}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hamiltonian" sheetId="1" r:id="rId1"/>
+    <sheet name="Analisis De T(n)" sheetId="1" r:id="rId1"/>
+    <sheet name="Pruebas" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">Hamiltonian!$B$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Hamiltonian!$B$3:$B$17</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Hamiltonian!$C$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Hamiltonian!$C$3:$C$17</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">Hamiltonian!$B$2</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">Hamiltonian!$B$3:$B$17</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">Hamiltonian!$C$2</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">Hamiltonian!$C$3:$C$17</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>Cantidad de Vertices</t>
   </si>
@@ -54,14 +45,35 @@
     <t>Caminos Posibles</t>
   </si>
   <si>
-    <t>Brute Force Method</t>
+    <t>Metodo Fuerza Bruta (Propio)</t>
+  </si>
+  <si>
+    <t>Metodo Fuerza Bruta (Comunidad)</t>
+  </si>
+  <si>
+    <t>Ejecución</t>
+  </si>
+  <si>
+    <t>Promedio</t>
+  </si>
+  <si>
+    <t>Cantidad de Vertices (Comunidad en Mac)</t>
+  </si>
+  <si>
+    <t>Cantidad de Vertices (Comunidad en Windows)</t>
+  </si>
+  <si>
+    <t>Cantidad de Vertices (Propio en Windows)</t>
+  </si>
+  <si>
+    <t>Cantidad de Vertices (Propio en Mac)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -76,8 +88,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,8 +114,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -129,11 +153,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -141,14 +189,43 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -247,7 +324,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hamiltonian!$C$2</c:f>
+              <c:f>'Analisis De T(n)'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -270,7 +347,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hamiltonian!$B$3:$B$17</c:f>
+              <c:f>'Analisis De T(n)'!$B$3:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -324,7 +401,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hamiltonian!$C$3:$C$17</c:f>
+              <c:f>'Analisis De T(n)'!$C$3:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -640,7 +717,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-HN"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -655,7 +732,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hamiltonian!$C$2</c:f>
+              <c:f>'Analisis De T(n)'!$C$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -678,7 +755,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Hamiltonian!$B$3:$B$10</c:f>
+              <c:f>'Analisis De T(n)'!$B$3:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -711,7 +788,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hamiltonian!$C$3:$C$10</c:f>
+              <c:f>'Analisis De T(n)'!$C$3:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -746,6 +823,775 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-41C5-0743-853C-B2968F5C4D9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1787797792"/>
+        <c:axId val="1607576304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1787797792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1607576304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1607576304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1787797792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-HN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Caminos Posibles Vista Exponencial</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-HN"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Analisis De T(n)'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caminos Posibles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Analisis De T(n)'!$B$3:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Analisis De T(n)'!$C$3:$C$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5040</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40320</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>362880</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3628800</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>39916800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>479001600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6227020800</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87178291200</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1307674368000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1D1-4A48-9459-E2A4D5FB5AD3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1787797792"/>
+        <c:axId val="1607576304"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1787797792"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1607576304"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1607576304"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-HN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1787797792"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-HN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Caminos Posibles Vista</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> de Punto de Inflexión</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Analisis De T(n)'!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Caminos Posibles</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Analisis De T(n)'!$B$3:$B$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Analisis De T(n)'!$C$3:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5040</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40320</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0468-C044-AC31-7A90AB53EBB4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1016,6 +1862,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1533,6 +2459,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2119,6 +4077,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>98592</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>187091</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>541978</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85491</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E39ADA-6A2A-2047-BA38-8E61FB4843D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>370661</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>199903</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>814047</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>98304</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF315A9E-53E0-A548-85E8-5159295876FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2444,10 +4478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BB1497-8041-B346-AE67-6F80C2596B26}">
-  <dimension ref="B2:O17"/>
+  <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2463,20 +4497,20 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
@@ -2486,18 +4520,18 @@
         <f>FACT(B3)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
@@ -2507,18 +4541,18 @@
         <f t="shared" ref="C4:C17" si="0">FACT(B4)</f>
         <v>2</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
@@ -2528,18 +4562,18 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
@@ -2549,18 +4583,18 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
@@ -2570,18 +4604,18 @@
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
@@ -2591,18 +4625,18 @@
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
@@ -2612,18 +4646,18 @@
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
@@ -2633,18 +4667,18 @@
         <f t="shared" si="0"/>
         <v>40320</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
@@ -2654,18 +4688,18 @@
         <f t="shared" si="0"/>
         <v>362880</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
@@ -2675,18 +4709,18 @@
         <f t="shared" si="0"/>
         <v>3628800</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
@@ -2696,18 +4730,18 @@
         <f t="shared" si="0"/>
         <v>39916800</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
@@ -2717,18 +4751,18 @@
         <f t="shared" si="0"/>
         <v>479001600</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
@@ -2738,18 +4772,18 @@
         <f t="shared" si="0"/>
         <v>6227020800</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-      <c r="O15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
@@ -2759,18 +4793,18 @@
         <f t="shared" si="0"/>
         <v>87178291200</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-      <c r="O16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
@@ -2780,25 +4814,1739 @@
         <f t="shared" si="0"/>
         <v>1307674368000</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-      <c r="O17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="2">
+        <f>FACT(B20)*B20</f>
+        <v>1</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <f>FACT(B21)*B21</f>
+        <v>4</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
+        <f t="shared" ref="C21:C34" si="1">FACT(B22)*B22</f>
+        <v>18</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B23" s="2">
+        <v>4</v>
+      </c>
+      <c r="C23" s="2">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+      <c r="D23" s="3"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="2">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B25" s="2">
+        <v>6</v>
+      </c>
+      <c r="C25" s="2">
+        <f t="shared" si="1"/>
+        <v>4320</v>
+      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="2">
+        <v>7</v>
+      </c>
+      <c r="C26" s="2">
+        <f t="shared" si="1"/>
+        <v>35280</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="2">
+        <v>8</v>
+      </c>
+      <c r="C27" s="2">
+        <f t="shared" si="1"/>
+        <v>322560</v>
+      </c>
+      <c r="D27" s="3"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="2">
+        <v>9</v>
+      </c>
+      <c r="C28" s="2">
+        <f t="shared" si="1"/>
+        <v>3265920</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>10</v>
+      </c>
+      <c r="C29" s="2">
+        <f t="shared" si="1"/>
+        <v>36288000</v>
+      </c>
+      <c r="D29" s="3"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <v>11</v>
+      </c>
+      <c r="C30" s="2">
+        <f t="shared" si="1"/>
+        <v>439084800</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="5"/>
+      <c r="I30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B31" s="2">
+        <v>12</v>
+      </c>
+      <c r="C31" s="2">
+        <f t="shared" si="1"/>
+        <v>5748019200</v>
+      </c>
+      <c r="D31" s="3"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B32" s="2">
+        <v>13</v>
+      </c>
+      <c r="C32" s="2">
+        <f t="shared" si="1"/>
+        <v>80951270400</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B33" s="2">
+        <v>14</v>
+      </c>
+      <c r="C33" s="2">
+        <f t="shared" si="1"/>
+        <v>1220496076800</v>
+      </c>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="B34" s="2">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2">
+        <f t="shared" si="1"/>
+        <v>19615115520000</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="D3:O17"/>
     <mergeCell ref="D2:O2"/>
+    <mergeCell ref="D19:O19"/>
+    <mergeCell ref="D20:O34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF4F965-C2D7-B34E-8DE3-F327C71C26E8}">
+  <dimension ref="B2:N39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="I2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6">
+        <v>5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12">
+        <v>12</v>
+      </c>
+      <c r="G3" s="9">
+        <v>13</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="6">
+        <v>5</v>
+      </c>
+      <c r="K3" s="6">
+        <v>7</v>
+      </c>
+      <c r="L3" s="6">
+        <v>10</v>
+      </c>
+      <c r="M3" s="12">
+        <v>12</v>
+      </c>
+      <c r="N3" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B4" s="16">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1.1019999999999999E-3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.56114699999999995</v>
+      </c>
+      <c r="F4" s="14">
+        <v>70.998412000000002</v>
+      </c>
+      <c r="G4" s="15">
+        <v>891.53199099999995</v>
+      </c>
+      <c r="I4" s="16">
+        <v>1</v>
+      </c>
+      <c r="J4" s="13">
+        <v>3.4E-5</v>
+      </c>
+      <c r="K4" s="13">
+        <v>2.7190000000000001E-3</v>
+      </c>
+      <c r="L4" s="13">
+        <v>0.61704199999999998</v>
+      </c>
+      <c r="M4" s="13">
+        <v>66.974783000000002</v>
+      </c>
+      <c r="N4" s="13">
+        <v>875.71974599999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B5" s="16">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13">
+        <v>3.4E-5</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1.0870000000000001E-3</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.59883799999999998</v>
+      </c>
+      <c r="F5" s="14">
+        <v>71.033137999999994</v>
+      </c>
+      <c r="G5" s="15">
+        <v>900.54676800000004</v>
+      </c>
+      <c r="I5" s="16">
+        <v>2</v>
+      </c>
+      <c r="J5" s="13">
+        <v>3.8000000000000002E-5</v>
+      </c>
+      <c r="K5" s="13">
+        <v>3.3219999999999999E-3</v>
+      </c>
+      <c r="L5" s="13">
+        <v>0.57754000000000005</v>
+      </c>
+      <c r="M5" s="13">
+        <v>67.261197999999993</v>
+      </c>
+      <c r="N5" s="13">
+        <v>859.53566699999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B6" s="16">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1.106E-3</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.59153900000000004</v>
+      </c>
+      <c r="F6" s="14">
+        <v>71.557794999999999</v>
+      </c>
+      <c r="G6" s="15">
+        <v>870.65565300000003</v>
+      </c>
+      <c r="I6" s="16">
+        <v>3</v>
+      </c>
+      <c r="J6" s="13">
+        <v>9.7999999999999997E-5</v>
+      </c>
+      <c r="K6" s="13">
+        <v>3.0430000000000001E-3</v>
+      </c>
+      <c r="L6" s="13">
+        <v>0.575797</v>
+      </c>
+      <c r="M6" s="13">
+        <v>67.517229999999998</v>
+      </c>
+      <c r="N6" s="13">
+        <v>899.44337800000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B7" s="16">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13">
+        <v>3.8000000000000002E-5</v>
+      </c>
+      <c r="D7" s="13">
+        <v>1.2210000000000001E-3</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.56531699999999996</v>
+      </c>
+      <c r="F7" s="14">
+        <v>70.761600000000001</v>
+      </c>
+      <c r="G7" s="15">
+        <v>859.94725400000004</v>
+      </c>
+      <c r="I7" s="16">
+        <v>4</v>
+      </c>
+      <c r="J7" s="13">
+        <v>9.1000000000000003E-5</v>
+      </c>
+      <c r="K7" s="13">
+        <v>2.9889999999999999E-3</v>
+      </c>
+      <c r="L7" s="13">
+        <v>0.57902900000000002</v>
+      </c>
+      <c r="M7" s="13">
+        <v>67.681213</v>
+      </c>
+      <c r="N7" s="13">
+        <v>907.43804299999999</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" s="16">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13">
+        <v>1.3100000000000001E-4</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1.08E-3</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.57264499999999996</v>
+      </c>
+      <c r="F8" s="14">
+        <v>67.707144999999997</v>
+      </c>
+      <c r="G8" s="15">
+        <v>882.92069500000002</v>
+      </c>
+      <c r="I8" s="16">
+        <v>5</v>
+      </c>
+      <c r="J8" s="13">
+        <v>1.03E-4</v>
+      </c>
+      <c r="K8" s="13">
+        <v>2.7820000000000002E-3</v>
+      </c>
+      <c r="L8" s="13">
+        <v>0.57530700000000001</v>
+      </c>
+      <c r="M8" s="13">
+        <v>67.671768</v>
+      </c>
+      <c r="N8" s="13">
+        <v>905.56920200000002</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B9" s="16">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="D9" s="13">
+        <v>1.1069999999999999E-3</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.59448000000000001</v>
+      </c>
+      <c r="F9" s="14">
+        <v>70.910909000000004</v>
+      </c>
+      <c r="G9" s="15">
+        <v>862.64565200000004</v>
+      </c>
+      <c r="I9" s="16">
+        <v>6</v>
+      </c>
+      <c r="J9" s="13">
+        <v>8.8999999999999995E-5</v>
+      </c>
+      <c r="K9" s="13">
+        <v>2.4229999999999998E-3</v>
+      </c>
+      <c r="L9" s="13">
+        <v>0.57561300000000004</v>
+      </c>
+      <c r="M9" s="13">
+        <v>67.699342999999999</v>
+      </c>
+      <c r="N9" s="13">
+        <v>904.69085500000006</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B10" s="16">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13">
+        <v>4.1999999999999998E-5</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.60327399999999998</v>
+      </c>
+      <c r="F10" s="14">
+        <v>67.652879999999996</v>
+      </c>
+      <c r="G10" s="15">
+        <v>900.16058599999997</v>
+      </c>
+      <c r="I10" s="16">
+        <v>7</v>
+      </c>
+      <c r="J10" s="13">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="K10" s="13">
+        <v>2.431E-3</v>
+      </c>
+      <c r="L10" s="13">
+        <v>0.58379899999999996</v>
+      </c>
+      <c r="M10" s="13">
+        <v>67.662175000000005</v>
+      </c>
+      <c r="N10" s="13">
+        <v>904.74132899999995</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B11" s="16">
+        <v>8</v>
+      </c>
+      <c r="C11" s="13">
+        <v>3.8000000000000002E-5</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1.175E-3</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.56802799999999998</v>
+      </c>
+      <c r="F11" s="14">
+        <v>71.371351000000004</v>
+      </c>
+      <c r="G11" s="15">
+        <v>892.77130699999998</v>
+      </c>
+      <c r="I11" s="16">
+        <v>8</v>
+      </c>
+      <c r="J11" s="13">
+        <v>8.5000000000000006E-5</v>
+      </c>
+      <c r="K11" s="13">
+        <v>2.5469999999999998E-3</v>
+      </c>
+      <c r="L11" s="13">
+        <v>0.57508000000000004</v>
+      </c>
+      <c r="M11" s="13">
+        <v>67.661006999999998</v>
+      </c>
+      <c r="N11" s="13">
+        <v>906.027244</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" s="16">
+        <v>9</v>
+      </c>
+      <c r="C12" s="13">
+        <v>3.4999999999999997E-5</v>
+      </c>
+      <c r="D12" s="13">
+        <v>9.9400000000000009E-4</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.59385299999999996</v>
+      </c>
+      <c r="F12" s="14">
+        <v>67.803026000000003</v>
+      </c>
+      <c r="G12" s="15">
+        <v>909.02992400000005</v>
+      </c>
+      <c r="I12" s="16">
+        <v>9</v>
+      </c>
+      <c r="J12" s="13">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="K12" s="13">
+        <v>2.4369999999999999E-3</v>
+      </c>
+      <c r="L12" s="13">
+        <v>0.58142799999999994</v>
+      </c>
+      <c r="M12" s="13">
+        <v>67.687242999999995</v>
+      </c>
+      <c r="N12" s="13">
+        <v>905.21150599999999</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="16">
+        <v>10</v>
+      </c>
+      <c r="C13" s="13">
+        <v>4.1E-5</v>
+      </c>
+      <c r="D13" s="13">
+        <v>9.990000000000001E-4</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.59433599999999998</v>
+      </c>
+      <c r="F13" s="14">
+        <v>71.812894999999997</v>
+      </c>
+      <c r="G13" s="15">
+        <v>884.195153</v>
+      </c>
+      <c r="I13" s="16">
+        <v>10</v>
+      </c>
+      <c r="J13" s="13">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="K13" s="13">
+        <v>2.1670000000000001E-3</v>
+      </c>
+      <c r="L13" s="13">
+        <v>0.57521699999999998</v>
+      </c>
+      <c r="M13" s="13">
+        <v>68.208561000000003</v>
+      </c>
+      <c r="N13" s="13">
+        <v>902.37817900000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" s="16">
+        <v>11</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="D14" s="13">
+        <v>1.06E-3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.591229</v>
+      </c>
+      <c r="F14" s="14">
+        <v>67.768906000000001</v>
+      </c>
+      <c r="G14" s="15">
+        <v>919.22993199999996</v>
+      </c>
+      <c r="I14" s="16">
+        <v>11</v>
+      </c>
+      <c r="J14" s="13">
+        <v>1.22E-4</v>
+      </c>
+      <c r="K14" s="13">
+        <v>2.1229999999999999E-3</v>
+      </c>
+      <c r="L14" s="13">
+        <v>0.57476099999999997</v>
+      </c>
+      <c r="M14" s="13">
+        <v>68.609347</v>
+      </c>
+      <c r="N14" s="13">
+        <v>904.03103299999998</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" s="16">
+        <v>12</v>
+      </c>
+      <c r="C15" s="13">
+        <v>8.6000000000000003E-5</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1.011E-3</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.56484900000000005</v>
+      </c>
+      <c r="F15" s="14">
+        <v>71.301658000000003</v>
+      </c>
+      <c r="G15" s="15">
+        <v>857.31556999999998</v>
+      </c>
+      <c r="I15" s="16">
+        <v>12</v>
+      </c>
+      <c r="J15" s="13">
+        <v>1.1E-4</v>
+      </c>
+      <c r="K15" s="13">
+        <v>2.1359999999999999E-3</v>
+      </c>
+      <c r="L15" s="13">
+        <v>0.57728599999999997</v>
+      </c>
+      <c r="M15" s="13">
+        <v>69.900491000000002</v>
+      </c>
+      <c r="N15" s="13">
+        <v>904.52477399999998</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" s="16">
+        <v>13</v>
+      </c>
+      <c r="C16" s="13">
+        <v>3.8000000000000002E-5</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1.018E-3</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.60061200000000003</v>
+      </c>
+      <c r="F16" s="14">
+        <v>70.395849999999996</v>
+      </c>
+      <c r="G16" s="15">
+        <v>897.37232200000005</v>
+      </c>
+      <c r="I16" s="16">
+        <v>13</v>
+      </c>
+      <c r="J16" s="13">
+        <v>1.08E-4</v>
+      </c>
+      <c r="K16" s="13">
+        <v>2.1120000000000002E-3</v>
+      </c>
+      <c r="L16" s="13">
+        <v>0.57594299999999998</v>
+      </c>
+      <c r="M16" s="13">
+        <v>69.574625999999995</v>
+      </c>
+      <c r="N16" s="13">
+        <v>902.913006</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B17" s="16">
+        <v>14</v>
+      </c>
+      <c r="C17" s="13">
+        <v>3.6000000000000001E-5</v>
+      </c>
+      <c r="D17" s="13">
+        <v>1.067E-3</v>
+      </c>
+      <c r="E17" s="13">
+        <v>0.59314500000000003</v>
+      </c>
+      <c r="F17" s="14">
+        <v>67.694800000000001</v>
+      </c>
+      <c r="G17" s="15">
+        <v>881.25936200000001</v>
+      </c>
+      <c r="I17" s="16">
+        <v>14</v>
+      </c>
+      <c r="J17" s="13">
+        <v>1.0900000000000001E-4</v>
+      </c>
+      <c r="K17" s="13">
+        <v>2.055E-3</v>
+      </c>
+      <c r="L17" s="13">
+        <v>0.58266200000000001</v>
+      </c>
+      <c r="M17" s="13">
+        <v>69.567784000000003</v>
+      </c>
+      <c r="N17" s="13">
+        <v>903.04707800000006</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B18" s="16">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13">
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="D18" s="13">
+        <v>1.023E-3</v>
+      </c>
+      <c r="E18" s="13">
+        <v>0.59454600000000002</v>
+      </c>
+      <c r="F18" s="14">
+        <v>67.169049999999999</v>
+      </c>
+      <c r="G18" s="15">
+        <v>883.04720399999997</v>
+      </c>
+      <c r="I18" s="16">
+        <v>15</v>
+      </c>
+      <c r="J18" s="13">
+        <v>1.13E-4</v>
+      </c>
+      <c r="K18" s="13">
+        <v>1.815E-3</v>
+      </c>
+      <c r="L18" s="13">
+        <v>0.57867299999999999</v>
+      </c>
+      <c r="M18" s="13">
+        <v>69.605817999999999</v>
+      </c>
+      <c r="N18" s="13">
+        <v>902.321325</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8">
+        <f>AVERAGE(C4:C18)</f>
+        <v>4.8266666666666677E-5</v>
+      </c>
+      <c r="D19" s="8">
+        <f t="shared" ref="D19:F19" si="0">AVERAGE(D4:D18)</f>
+        <v>1.0730000000000002E-3</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.58585586666666656</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="0"/>
+        <v>69.729294333333343</v>
+      </c>
+      <c r="G19" s="8">
+        <f>AVERAGE(G4:G18)</f>
+        <v>886.17529153333339</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="8">
+        <f>AVERAGE(J4:J18)</f>
+        <v>9.0533333333333343E-5</v>
+      </c>
+      <c r="K19" s="8">
+        <f t="shared" ref="K19" si="1">AVERAGE(K4:K18)</f>
+        <v>2.4733999999999997E-3</v>
+      </c>
+      <c r="L19" s="8">
+        <f t="shared" ref="L19" si="2">AVERAGE(L4:L18)</f>
+        <v>0.58034513333333337</v>
+      </c>
+      <c r="M19" s="8">
+        <f t="shared" ref="M19" si="3">AVERAGE(M4:M18)</f>
+        <v>68.218839133333319</v>
+      </c>
+      <c r="N19" s="8">
+        <f t="shared" ref="N19" si="4">AVERAGE(N4:N18)</f>
+        <v>899.17282433333321</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="I22" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="6">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>7</v>
+      </c>
+      <c r="E23" s="6">
+        <v>10</v>
+      </c>
+      <c r="F23" s="12">
+        <v>12</v>
+      </c>
+      <c r="G23" s="9">
+        <v>13</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23" s="6">
+        <v>5</v>
+      </c>
+      <c r="K23" s="6">
+        <v>7</v>
+      </c>
+      <c r="L23" s="6">
+        <v>10</v>
+      </c>
+      <c r="M23" s="12">
+        <v>12</v>
+      </c>
+      <c r="N23" s="9">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B24" s="16">
+        <v>1</v>
+      </c>
+      <c r="C24" s="13">
+        <v>0</v>
+      </c>
+      <c r="D24" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E24" s="13">
+        <v>0.58099999999999996</v>
+      </c>
+      <c r="F24" s="13">
+        <v>77.986999999999995</v>
+      </c>
+      <c r="G24" s="13">
+        <v>859.81700000000001</v>
+      </c>
+      <c r="I24" s="16">
+        <v>1</v>
+      </c>
+      <c r="J24" s="13">
+        <v>0</v>
+      </c>
+      <c r="K24" s="13">
+        <v>0</v>
+      </c>
+      <c r="L24" s="13">
+        <v>0</v>
+      </c>
+      <c r="M24" s="13">
+        <v>0</v>
+      </c>
+      <c r="N24" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B25" s="16">
+        <v>2</v>
+      </c>
+      <c r="C25" s="13">
+        <v>0</v>
+      </c>
+      <c r="D25" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E25" s="13">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F25" s="13">
+        <v>77.272999999999996</v>
+      </c>
+      <c r="G25" s="13">
+        <v>857.47</v>
+      </c>
+      <c r="I25" s="16">
+        <v>2</v>
+      </c>
+      <c r="J25" s="13">
+        <v>0</v>
+      </c>
+      <c r="K25" s="13">
+        <v>0</v>
+      </c>
+      <c r="L25" s="13">
+        <v>0</v>
+      </c>
+      <c r="M25" s="13">
+        <v>0</v>
+      </c>
+      <c r="N25" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B26" s="16">
+        <v>3</v>
+      </c>
+      <c r="C26" s="13">
+        <v>0</v>
+      </c>
+      <c r="D26" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E26" s="13">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="F26" s="13">
+        <v>76.853999999999999</v>
+      </c>
+      <c r="G26" s="13">
+        <v>854.726</v>
+      </c>
+      <c r="I26" s="16">
+        <v>3</v>
+      </c>
+      <c r="J26" s="13">
+        <v>0</v>
+      </c>
+      <c r="K26" s="13">
+        <v>0</v>
+      </c>
+      <c r="L26" s="13">
+        <v>0</v>
+      </c>
+      <c r="M26" s="13">
+        <v>0</v>
+      </c>
+      <c r="N26" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B27" s="16">
+        <v>4</v>
+      </c>
+      <c r="C27" s="13">
+        <v>0</v>
+      </c>
+      <c r="D27" s="13">
+        <v>0</v>
+      </c>
+      <c r="E27" s="13">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F27" s="13">
+        <v>79.584999999999994</v>
+      </c>
+      <c r="G27" s="13">
+        <v>859.99599999999998</v>
+      </c>
+      <c r="I27" s="16">
+        <v>4</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="13">
+        <v>0</v>
+      </c>
+      <c r="L27" s="13">
+        <v>0</v>
+      </c>
+      <c r="M27" s="13">
+        <v>0</v>
+      </c>
+      <c r="N27" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B28" s="16">
+        <v>5</v>
+      </c>
+      <c r="C28" s="13">
+        <v>0</v>
+      </c>
+      <c r="D28" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E28" s="13">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="F28" s="13">
+        <v>77.947999999999993</v>
+      </c>
+      <c r="G28" s="13">
+        <v>919.50800000000004</v>
+      </c>
+      <c r="I28" s="16">
+        <v>5</v>
+      </c>
+      <c r="J28" s="13">
+        <v>0</v>
+      </c>
+      <c r="K28" s="13">
+        <v>0</v>
+      </c>
+      <c r="L28" s="13">
+        <v>0</v>
+      </c>
+      <c r="M28" s="13">
+        <v>0</v>
+      </c>
+      <c r="N28" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29" s="16">
+        <v>6</v>
+      </c>
+      <c r="C29" s="13">
+        <v>0</v>
+      </c>
+      <c r="D29" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E29" s="13">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="F29" s="13">
+        <v>73.369</v>
+      </c>
+      <c r="G29" s="13">
+        <v>949.37</v>
+      </c>
+      <c r="I29" s="16">
+        <v>6</v>
+      </c>
+      <c r="J29" s="13">
+        <v>0</v>
+      </c>
+      <c r="K29" s="13">
+        <v>0</v>
+      </c>
+      <c r="L29" s="13">
+        <v>0</v>
+      </c>
+      <c r="M29" s="13">
+        <v>0</v>
+      </c>
+      <c r="N29" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30" s="16">
+        <v>7</v>
+      </c>
+      <c r="C30" s="13">
+        <v>0</v>
+      </c>
+      <c r="D30" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E30" s="13">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F30" s="13">
+        <v>67.111999999999995</v>
+      </c>
+      <c r="G30" s="13">
+        <v>993.71299999999997</v>
+      </c>
+      <c r="I30" s="16">
+        <v>7</v>
+      </c>
+      <c r="J30" s="13">
+        <v>0</v>
+      </c>
+      <c r="K30" s="13">
+        <v>0</v>
+      </c>
+      <c r="L30" s="13">
+        <v>0</v>
+      </c>
+      <c r="M30" s="13">
+        <v>0</v>
+      </c>
+      <c r="N30" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" s="16">
+        <v>8</v>
+      </c>
+      <c r="C31" s="13">
+        <v>0</v>
+      </c>
+      <c r="D31" s="13">
+        <v>0</v>
+      </c>
+      <c r="E31" s="13">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F31" s="13">
+        <v>66.84</v>
+      </c>
+      <c r="G31" s="13">
+        <v>1039.277</v>
+      </c>
+      <c r="I31" s="16">
+        <v>8</v>
+      </c>
+      <c r="J31" s="13">
+        <v>0</v>
+      </c>
+      <c r="K31" s="13">
+        <v>0</v>
+      </c>
+      <c r="L31" s="13">
+        <v>0</v>
+      </c>
+      <c r="M31" s="13">
+        <v>0</v>
+      </c>
+      <c r="N31" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="16">
+        <v>9</v>
+      </c>
+      <c r="C32" s="13">
+        <v>0</v>
+      </c>
+      <c r="D32" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="E32" s="13">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F32" s="13">
+        <v>67.522000000000006</v>
+      </c>
+      <c r="G32" s="13">
+        <v>969.779</v>
+      </c>
+      <c r="I32" s="16">
+        <v>9</v>
+      </c>
+      <c r="J32" s="13">
+        <v>0</v>
+      </c>
+      <c r="K32" s="13">
+        <v>0</v>
+      </c>
+      <c r="L32" s="13">
+        <v>0</v>
+      </c>
+      <c r="M32" s="13">
+        <v>0</v>
+      </c>
+      <c r="N32" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B33" s="16">
+        <v>10</v>
+      </c>
+      <c r="C33" s="13">
+        <v>0</v>
+      </c>
+      <c r="D33" s="13">
+        <v>0</v>
+      </c>
+      <c r="E33" s="13">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="F33" s="13">
+        <v>67.322000000000003</v>
+      </c>
+      <c r="G33" s="13">
+        <v>1426.3309999999999</v>
+      </c>
+      <c r="I33" s="16">
+        <v>10</v>
+      </c>
+      <c r="J33" s="13">
+        <v>0</v>
+      </c>
+      <c r="K33" s="13">
+        <v>0</v>
+      </c>
+      <c r="L33" s="13">
+        <v>0</v>
+      </c>
+      <c r="M33" s="13">
+        <v>0</v>
+      </c>
+      <c r="N33" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="16">
+        <v>11</v>
+      </c>
+      <c r="C34" s="13">
+        <v>0</v>
+      </c>
+      <c r="D34" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="E34" s="13">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F34" s="13">
+        <v>68.34</v>
+      </c>
+      <c r="G34" s="13">
+        <v>880.62599999999998</v>
+      </c>
+      <c r="I34" s="16">
+        <v>11</v>
+      </c>
+      <c r="J34" s="13">
+        <v>0</v>
+      </c>
+      <c r="K34" s="13">
+        <v>0</v>
+      </c>
+      <c r="L34" s="13">
+        <v>0</v>
+      </c>
+      <c r="M34" s="13">
+        <v>0</v>
+      </c>
+      <c r="N34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="16">
+        <v>12</v>
+      </c>
+      <c r="C35" s="13">
+        <v>0</v>
+      </c>
+      <c r="D35" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E35" s="13">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="F35" s="13">
+        <v>66.381</v>
+      </c>
+      <c r="G35" s="13">
+        <v>909.29200000000003</v>
+      </c>
+      <c r="I35" s="16">
+        <v>12</v>
+      </c>
+      <c r="J35" s="13">
+        <v>0</v>
+      </c>
+      <c r="K35" s="13">
+        <v>0</v>
+      </c>
+      <c r="L35" s="13">
+        <v>0</v>
+      </c>
+      <c r="M35" s="13">
+        <v>0</v>
+      </c>
+      <c r="N35" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="16">
+        <v>13</v>
+      </c>
+      <c r="C36" s="13">
+        <v>0</v>
+      </c>
+      <c r="D36" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E36" s="13">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="F36" s="13">
+        <v>65.631</v>
+      </c>
+      <c r="G36" s="13">
+        <v>902.40099999999995</v>
+      </c>
+      <c r="I36" s="16">
+        <v>13</v>
+      </c>
+      <c r="J36" s="13">
+        <v>0</v>
+      </c>
+      <c r="K36" s="13">
+        <v>0</v>
+      </c>
+      <c r="L36" s="13">
+        <v>0</v>
+      </c>
+      <c r="M36" s="13">
+        <v>0</v>
+      </c>
+      <c r="N36" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B37" s="16">
+        <v>14</v>
+      </c>
+      <c r="C37" s="13">
+        <v>0</v>
+      </c>
+      <c r="D37" s="13">
+        <v>2E-3</v>
+      </c>
+      <c r="E37" s="13">
+        <v>0.54700000000000004</v>
+      </c>
+      <c r="F37" s="13">
+        <v>65.620999999999995</v>
+      </c>
+      <c r="G37" s="13">
+        <v>901.55899999999997</v>
+      </c>
+      <c r="I37" s="16">
+        <v>14</v>
+      </c>
+      <c r="J37" s="13">
+        <v>0</v>
+      </c>
+      <c r="K37" s="13">
+        <v>0</v>
+      </c>
+      <c r="L37" s="13">
+        <v>0</v>
+      </c>
+      <c r="M37" s="13">
+        <v>0</v>
+      </c>
+      <c r="N37" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B38" s="16">
+        <v>15</v>
+      </c>
+      <c r="C38" s="13">
+        <v>0</v>
+      </c>
+      <c r="D38" s="13">
+        <v>1E-3</v>
+      </c>
+      <c r="E38" s="13">
+        <v>0.60699999999999998</v>
+      </c>
+      <c r="F38" s="13">
+        <v>65.831999999999994</v>
+      </c>
+      <c r="G38" s="13">
+        <v>900.37400000000002</v>
+      </c>
+      <c r="I38" s="16">
+        <v>15</v>
+      </c>
+      <c r="J38" s="13">
+        <v>0</v>
+      </c>
+      <c r="K38" s="13">
+        <v>0</v>
+      </c>
+      <c r="L38" s="13">
+        <v>0</v>
+      </c>
+      <c r="M38" s="13">
+        <v>0</v>
+      </c>
+      <c r="N38" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="8">
+        <f>AVERAGE(C24:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="8">
+        <f t="shared" ref="D39" si="5">AVERAGE(D24:D38)</f>
+        <v>1E-3</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" ref="E39" si="6">AVERAGE(E24:E38)</f>
+        <v>0.59906666666666664</v>
+      </c>
+      <c r="F39" s="8">
+        <f t="shared" ref="F39" si="7">AVERAGE(F24:F38)</f>
+        <v>70.907799999999995</v>
+      </c>
+      <c r="G39" s="8">
+        <f t="shared" ref="G39" si="8">AVERAGE(G24:G38)</f>
+        <v>948.28259999999989</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J39" s="8">
+        <f>AVERAGE(J24:J38)</f>
+        <v>0</v>
+      </c>
+      <c r="K39" s="8">
+        <f t="shared" ref="K39" si="9">AVERAGE(K24:K38)</f>
+        <v>0</v>
+      </c>
+      <c r="L39" s="8">
+        <f t="shared" ref="L39" si="10">AVERAGE(L24:L38)</f>
+        <v>0</v>
+      </c>
+      <c r="M39" s="8">
+        <f t="shared" ref="M39" si="11">AVERAGE(M24:M38)</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="8">
+        <f t="shared" ref="N39" si="12">AVERAGE(N24:N38)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="B22:G22"/>
+    <mergeCell ref="I22:N22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio en devolver el grafo original
</commit_message>
<xml_diff>
--- a/Analisis de Cantidad de Vertices.xlsx
+++ b/Analisis de Cantidad de Vertices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dan29reyes/Desktop/analisis_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5082FC0A-8265-EA41-9CBF-EFA124CC4D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F320FAB5-A4A4-2C4A-A552-6AD50DA32E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="620" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{36B05C6E-00E7-8741-8E22-DAB7CBFD8F63}"/>
+    <workbookView xWindow="0" yWindow="620" windowWidth="28800" windowHeight="16120" activeTab="1" xr2:uid="{36B05C6E-00E7-8741-8E22-DAB7CBFD8F63}"/>
   </bookViews>
   <sheets>
     <sheet name="Analisis De T(n)" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Cantidad de Vertices</t>
   </si>
@@ -68,12 +68,40 @@
   <si>
     <t>Cantidad de Vertices (Propio en Mac)</t>
   </si>
+  <si>
+    <t>67..757</t>
+  </si>
+  <si>
+    <t>Tiempo Esperado en Base al Promedio</t>
+  </si>
+  <si>
+    <t>Vertices</t>
+  </si>
+  <si>
+    <t>Propio Mac</t>
+  </si>
+  <si>
+    <t>Propio Windows</t>
+  </si>
+  <si>
+    <t>Comunidad Mac</t>
+  </si>
+  <si>
+    <t>Comunidad Windows</t>
+  </si>
+  <si>
+    <t>Tiempo en seg Por Permutación</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,6 +120,13 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -121,7 +156,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -177,11 +212,36 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,46 +249,56 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -403,7 +473,7 @@
             <c:numRef>
               <c:f>'Analisis De T(n)'!$C$3:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -554,7 +624,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -790,7 +860,7 @@
             <c:numRef>
               <c:f>'Analisis De T(n)'!$C$3:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -920,7 +990,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1116,7 +1186,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Analisis De T(n)'!$B$3:$B$17</c:f>
+              <c:f>'Analisis De T(n)'!$B$20:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1170,9 +1240,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Analisis De T(n)'!$C$3:$C$17</c:f>
+              <c:f>'Analisis De T(n)'!$C$20:$C$34</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -1323,7 +1393,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1524,7 +1594,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Analisis De T(n)'!$B$3:$B$10</c:f>
+              <c:f>'Analisis De T(n)'!$B$20:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1557,9 +1627,9 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Analisis De T(n)'!$C$3:$C$10</c:f>
+              <c:f>'Analisis De T(n)'!$C$20:$C$27</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
@@ -1689,7 +1759,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4480,14 +4550,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4BB1497-8041-B346-AE67-6F80C2596B26}">
   <dimension ref="B2:O34"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.2">
@@ -4497,335 +4567,335 @@
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="14">
         <f>FACT(B3)</f>
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="14">
         <f t="shared" ref="C4:C17" si="0">FACT(B4)</f>
         <v>2</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="2">
         <v>3</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="14">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="2">
         <v>4</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="14">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="2">
         <v>5</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="14">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="2">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="14">
         <f t="shared" si="0"/>
         <v>720</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="2">
         <v>7</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="14">
         <f t="shared" si="0"/>
         <v>5040</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="2">
         <v>8</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="14">
         <f t="shared" si="0"/>
         <v>40320</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="2">
         <v>9</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="14">
         <f t="shared" si="0"/>
         <v>362880</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="14">
         <f t="shared" si="0"/>
         <v>3628800</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="2">
         <v>11</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="14">
         <f t="shared" si="0"/>
         <v>39916800</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="2">
         <v>12</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="14">
         <f t="shared" si="0"/>
         <v>479001600</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="2">
         <v>13</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="14">
         <f t="shared" si="0"/>
         <v>6227020800</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="2">
         <v>14</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="14">
         <f t="shared" si="0"/>
         <v>87178291200</v>
       </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B17" s="2">
         <v>15</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="14">
         <f t="shared" si="0"/>
         <v>1307674368000</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
@@ -4834,335 +4904,335 @@
       <c r="C19" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="D19" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
-      <c r="O19" s="4"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>1</v>
       </c>
-      <c r="C20" s="2">
-        <f>FACT(B20)*B20</f>
+      <c r="C20" s="14">
+        <f>FACT(B20)</f>
         <v>1</v>
       </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="10"/>
+      <c r="J20" s="10"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>2</v>
       </c>
-      <c r="C21" s="2">
-        <f>FACT(B21)*B21</f>
-        <v>4</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="C21" s="14">
+        <f t="shared" ref="C21:C34" si="1">FACT(B21)</f>
+        <v>2</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="10"/>
+      <c r="J21" s="10"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
+      <c r="N21" s="10"/>
+      <c r="O21" s="10"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>3</v>
       </c>
-      <c r="C22" s="2">
-        <f t="shared" ref="C21:C34" si="1">FACT(B22)*B22</f>
-        <v>18</v>
-      </c>
-      <c r="D22" s="3"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
+      <c r="C22" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="10"/>
+      <c r="O22" s="10"/>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B23" s="2">
         <v>4</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="14">
         <f t="shared" si="1"/>
-        <v>96</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="D23" s="9"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="10"/>
+      <c r="N23" s="10"/>
+      <c r="O23" s="10"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B24" s="2">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="14">
         <f t="shared" si="1"/>
-        <v>600</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+        <v>120</v>
+      </c>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="10"/>
+      <c r="N24" s="10"/>
+      <c r="O24" s="10"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B25" s="2">
         <v>6</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="14">
         <f t="shared" si="1"/>
-        <v>4320</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+        <v>720</v>
+      </c>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B26" s="2">
         <v>7</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="14">
         <f t="shared" si="1"/>
-        <v>35280</v>
-      </c>
-      <c r="D26" s="3"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+        <v>5040</v>
+      </c>
+      <c r="D26" s="9"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="10"/>
+      <c r="G26" s="10"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="10"/>
+      <c r="J26" s="10"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
+      <c r="N26" s="10"/>
+      <c r="O26" s="10"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B27" s="2">
         <v>8</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="14">
         <f t="shared" si="1"/>
-        <v>322560</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+        <v>40320</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="10"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="10"/>
+      <c r="I27" s="10"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="10"/>
+      <c r="M27" s="10"/>
+      <c r="N27" s="10"/>
+      <c r="O27" s="10"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B28" s="2">
         <v>9</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="14">
         <f t="shared" si="1"/>
-        <v>3265920</v>
-      </c>
-      <c r="D28" s="3"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
+        <v>362880</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
+      <c r="N28" s="10"/>
+      <c r="O28" s="10"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B29" s="2">
         <v>10</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="14">
         <f t="shared" si="1"/>
-        <v>36288000</v>
-      </c>
-      <c r="D29" s="3"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
+        <v>3628800</v>
+      </c>
+      <c r="D29" s="9"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
+      <c r="K29" s="10"/>
+      <c r="L29" s="10"/>
+      <c r="M29" s="10"/>
+      <c r="N29" s="10"/>
+      <c r="O29" s="10"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B30" s="2">
         <v>11</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="14">
         <f t="shared" si="1"/>
-        <v>439084800</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
+        <v>39916800</v>
+      </c>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
+      <c r="K30" s="10"/>
+      <c r="L30" s="10"/>
+      <c r="M30" s="10"/>
+      <c r="N30" s="10"/>
+      <c r="O30" s="10"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B31" s="2">
         <v>12</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="14">
         <f t="shared" si="1"/>
-        <v>5748019200</v>
-      </c>
-      <c r="D31" s="3"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
+        <v>479001600</v>
+      </c>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="10"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="10"/>
+      <c r="K31" s="10"/>
+      <c r="L31" s="10"/>
+      <c r="M31" s="10"/>
+      <c r="N31" s="10"/>
+      <c r="O31" s="10"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B32" s="2">
         <v>13</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="14">
         <f t="shared" si="1"/>
-        <v>80951270400</v>
-      </c>
-      <c r="D32" s="3"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
+        <v>6227020800</v>
+      </c>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="10"/>
+      <c r="J32" s="10"/>
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="10"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B33" s="2">
         <v>14</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="14">
         <f t="shared" si="1"/>
-        <v>1220496076800</v>
-      </c>
-      <c r="D33" s="3"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
+        <v>87178291200</v>
+      </c>
+      <c r="D33" s="9"/>
+      <c r="E33" s="10"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="10"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="10"/>
+      <c r="J33" s="10"/>
+      <c r="K33" s="10"/>
+      <c r="L33" s="10"/>
+      <c r="M33" s="10"/>
+      <c r="N33" s="10"/>
+      <c r="O33" s="10"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B34" s="2">
         <v>15</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="14">
         <f t="shared" si="1"/>
-        <v>19615115520000</v>
-      </c>
-      <c r="D34" s="3"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
+        <v>1307674368000</v>
+      </c>
+      <c r="D34" s="9"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="10"/>
+      <c r="J34" s="10"/>
+      <c r="K34" s="10"/>
+      <c r="L34" s="10"/>
+      <c r="M34" s="10"/>
+      <c r="N34" s="10"/>
+      <c r="O34" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5178,10 +5248,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF4F965-C2D7-B34E-8DE3-F327C71C26E8}">
-  <dimension ref="B2:N39"/>
+  <dimension ref="B2:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5190,1358 +5260,1708 @@
     <col min="4" max="4" width="11" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="I2" s="10" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="I2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="P2" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" s="17"/>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="3">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>7</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="3">
         <v>10</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="6">
         <v>12</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <v>13</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="3">
         <v>5</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="3">
         <v>7</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="3">
         <v>10</v>
       </c>
-      <c r="M3" s="12">
+      <c r="M3" s="6">
         <v>12</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="5">
         <v>13</v>
       </c>
+      <c r="P3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="2">
+        <f>G19/FACT(13)</f>
+        <v>1.4231127853841976E-7</v>
+      </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="16">
+    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="2">
         <v>3.6000000000000001E-5</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="2">
         <v>1.1019999999999999E-3</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="2">
         <v>0.56114699999999995</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="7">
         <v>70.998412000000002</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="8">
         <v>891.53199099999995</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="2">
         <v>1</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="2">
         <v>3.4E-5</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="2">
         <v>2.7190000000000001E-3</v>
       </c>
-      <c r="L4" s="13">
+      <c r="L4" s="2">
         <v>0.61704199999999998</v>
       </c>
-      <c r="M4" s="13">
+      <c r="M4" s="2">
         <v>66.974783000000002</v>
       </c>
-      <c r="N4" s="13">
+      <c r="N4" s="2">
         <v>875.71974599999999</v>
       </c>
+      <c r="P4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="2">
+        <f>G39/FACT(13)</f>
+        <v>1.5228511843095175E-7</v>
+      </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="16">
+    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
         <v>2</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="2">
         <v>3.4E-5</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="2">
         <v>1.0870000000000001E-3</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="2">
         <v>0.59883799999999998</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="7">
         <v>71.033137999999994</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="8">
         <v>900.54676800000004</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="2">
         <v>2</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="2">
         <v>3.8000000000000002E-5</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="2">
         <v>3.3219999999999999E-3</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="2">
         <v>0.57754000000000005</v>
       </c>
-      <c r="M5" s="13">
+      <c r="M5" s="2">
         <v>67.261197999999993</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="2">
         <v>859.53566699999999</v>
       </c>
+      <c r="P5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q5" s="2">
+        <f>N19/FACT(13)</f>
+        <v>1.4439855802847699E-7</v>
+      </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="16">
+    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="2">
         <v>4.1999999999999998E-5</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="2">
         <v>1.106E-3</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="2">
         <v>0.59153900000000004</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="7">
         <v>71.557794999999999</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="8">
         <v>870.65565300000003</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="2">
         <v>3</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="2">
         <v>9.7999999999999997E-5</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="2">
         <v>3.0430000000000001E-3</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="2">
         <v>0.575797</v>
       </c>
-      <c r="M6" s="13">
+      <c r="M6" s="2">
         <v>67.517229999999998</v>
       </c>
-      <c r="N6" s="13">
+      <c r="N6" s="2">
         <v>899.44337800000005</v>
       </c>
+      <c r="P6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q6" s="2">
+        <f>N39/FACT(13)</f>
+        <v>1.4073595728688323E-7</v>
+      </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="16">
+    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B7" s="2">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="2">
         <v>3.8000000000000002E-5</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="2">
         <v>1.2210000000000001E-3</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="2">
         <v>0.56531699999999996</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="7">
         <v>70.761600000000001</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="8">
         <v>859.94725400000004</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="2">
         <v>4</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="2">
         <v>9.1000000000000003E-5</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="2">
         <v>2.9889999999999999E-3</v>
       </c>
-      <c r="L7" s="13">
+      <c r="L7" s="2">
         <v>0.57902900000000002</v>
       </c>
-      <c r="M7" s="13">
+      <c r="M7" s="2">
         <v>67.681213</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="2">
         <v>907.43804299999999</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="16">
+    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B8" s="2">
         <v>5</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="2">
         <v>1.3100000000000001E-4</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="2">
         <v>1.08E-3</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="2">
         <v>0.57264499999999996</v>
       </c>
-      <c r="F8" s="14">
+      <c r="F8" s="7">
         <v>67.707144999999997</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="8">
         <v>882.92069500000002</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="2">
         <v>5</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="2">
         <v>1.03E-4</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="2">
         <v>2.7820000000000002E-3</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="2">
         <v>0.57530700000000001</v>
       </c>
-      <c r="M8" s="13">
+      <c r="M8" s="2">
         <v>67.671768</v>
       </c>
-      <c r="N8" s="13">
+      <c r="N8" s="2">
         <v>905.56920200000002</v>
       </c>
+      <c r="P8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="16">
+    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B9" s="2">
         <v>6</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="2">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="2">
         <v>1.1069999999999999E-3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="2">
         <v>0.59448000000000001</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="7">
         <v>70.910909000000004</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="8">
         <v>862.64565200000004</v>
       </c>
-      <c r="I9" s="16">
+      <c r="I9" s="2">
         <v>6</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="2">
         <v>8.8999999999999995E-5</v>
       </c>
-      <c r="K9" s="13">
+      <c r="K9" s="2">
         <v>2.4229999999999998E-3</v>
       </c>
-      <c r="L9" s="13">
+      <c r="L9" s="2">
         <v>0.57561300000000004</v>
       </c>
-      <c r="M9" s="13">
+      <c r="M9" s="2">
         <v>67.699342999999999</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="2">
         <v>904.69085500000006</v>
       </c>
+      <c r="P9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="16">
+    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B10" s="2">
         <v>7</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="2">
         <v>4.1999999999999998E-5</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="2">
         <v>1.0449999999999999E-3</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="2">
         <v>0.60327399999999998</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="7">
         <v>67.652879999999996</v>
       </c>
-      <c r="G10" s="15">
+      <c r="G10" s="8">
         <v>900.16058599999997</v>
       </c>
-      <c r="I10" s="16">
+      <c r="I10" s="2">
         <v>7</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="2">
         <v>8.6000000000000003E-5</v>
       </c>
-      <c r="K10" s="13">
+      <c r="K10" s="2">
         <v>2.431E-3</v>
       </c>
-      <c r="L10" s="13">
+      <c r="L10" s="2">
         <v>0.58379899999999996</v>
       </c>
-      <c r="M10" s="13">
+      <c r="M10" s="2">
         <v>67.662175000000005</v>
       </c>
-      <c r="N10" s="13">
+      <c r="N10" s="2">
         <v>904.74132899999995</v>
       </c>
+      <c r="P10" s="19">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <f t="shared" ref="Q10:Q14" si="0">$Q$3*FACT(P10)</f>
+        <v>1.4231127853841976E-7</v>
+      </c>
+      <c r="R10" s="2">
+        <f t="shared" ref="R10:R14" si="1">$Q$4*FACT(P10)</f>
+        <v>1.5228511843095175E-7</v>
+      </c>
+      <c r="S10" s="2">
+        <f t="shared" ref="S10:S14" si="2">$Q$5*FACT(P10)</f>
+        <v>1.4439855802847699E-7</v>
+      </c>
+      <c r="T10" s="15">
+        <f t="shared" ref="T10:T14" si="3">$Q$6*FACT(P10)</f>
+        <v>1.4073595728688323E-7</v>
+      </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="16">
+    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B11" s="2">
         <v>8</v>
       </c>
-      <c r="C11" s="13">
+      <c r="C11" s="2">
         <v>3.8000000000000002E-5</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="2">
         <v>1.175E-3</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="2">
         <v>0.56802799999999998</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="7">
         <v>71.371351000000004</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="8">
         <v>892.77130699999998</v>
       </c>
-      <c r="I11" s="16">
+      <c r="I11" s="2">
         <v>8</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="2">
         <v>8.5000000000000006E-5</v>
       </c>
-      <c r="K11" s="13">
+      <c r="K11" s="2">
         <v>2.5469999999999998E-3</v>
       </c>
-      <c r="L11" s="13">
+      <c r="L11" s="2">
         <v>0.57508000000000004</v>
       </c>
-      <c r="M11" s="13">
+      <c r="M11" s="2">
         <v>67.661006999999998</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="2">
         <v>906.027244</v>
       </c>
+      <c r="P11" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="2">
+        <f t="shared" si="0"/>
+        <v>2.8462255707683952E-7</v>
+      </c>
+      <c r="R11" s="2">
+        <f t="shared" si="1"/>
+        <v>3.045702368619035E-7</v>
+      </c>
+      <c r="S11" s="2">
+        <f t="shared" si="2"/>
+        <v>2.8879711605695398E-7</v>
+      </c>
+      <c r="T11" s="15">
+        <f>$Q$6*FACT(P11)</f>
+        <v>2.8147191457376646E-7</v>
+      </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="16">
+    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
         <v>9</v>
       </c>
-      <c r="C12" s="13">
+      <c r="C12" s="2">
         <v>3.4999999999999997E-5</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="2">
         <v>9.9400000000000009E-4</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E12" s="2">
         <v>0.59385299999999996</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="7">
         <v>67.803026000000003</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G12" s="8">
         <v>909.02992400000005</v>
       </c>
-      <c r="I12" s="16">
+      <c r="I12" s="2">
         <v>9</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="2">
         <v>8.6000000000000003E-5</v>
       </c>
-      <c r="K12" s="13">
+      <c r="K12" s="2">
         <v>2.4369999999999999E-3</v>
       </c>
-      <c r="L12" s="13">
+      <c r="L12" s="2">
         <v>0.58142799999999994</v>
       </c>
-      <c r="M12" s="13">
+      <c r="M12" s="2">
         <v>67.687242999999995</v>
       </c>
-      <c r="N12" s="13">
+      <c r="N12" s="2">
         <v>905.21150599999999</v>
       </c>
+      <c r="P12" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="2">
+        <f t="shared" si="0"/>
+        <v>8.5386767123051856E-7</v>
+      </c>
+      <c r="R12" s="2">
+        <f t="shared" si="1"/>
+        <v>9.137107105857105E-7</v>
+      </c>
+      <c r="S12" s="2">
+        <f t="shared" si="2"/>
+        <v>8.6639134817086193E-7</v>
+      </c>
+      <c r="T12" s="15">
+        <f t="shared" si="3"/>
+        <v>8.4441574372129933E-7</v>
+      </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="16">
+    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
         <v>10</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="2">
         <v>4.1E-5</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="2">
         <v>9.990000000000001E-4</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="2">
         <v>0.59433599999999998</v>
       </c>
-      <c r="F13" s="14">
+      <c r="F13" s="7">
         <v>71.812894999999997</v>
       </c>
-      <c r="G13" s="15">
+      <c r="G13" s="8">
         <v>884.195153</v>
       </c>
-      <c r="I13" s="16">
+      <c r="I13" s="2">
         <v>10</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="2">
         <v>8.6000000000000003E-5</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K13" s="2">
         <v>2.1670000000000001E-3</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L13" s="2">
         <v>0.57521699999999998</v>
       </c>
-      <c r="M13" s="13">
+      <c r="M13" s="2">
         <v>68.208561000000003</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="2">
         <v>902.37817900000005</v>
       </c>
+      <c r="P13" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="2">
+        <f t="shared" si="0"/>
+        <v>3.4154706849220743E-6</v>
+      </c>
+      <c r="R13" s="2">
+        <f t="shared" si="1"/>
+        <v>3.654842842342842E-6</v>
+      </c>
+      <c r="S13" s="2">
+        <f t="shared" si="2"/>
+        <v>3.4655653926834477E-6</v>
+      </c>
+      <c r="T13" s="15">
+        <f t="shared" si="3"/>
+        <v>3.3776629748851973E-6</v>
+      </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="16">
+    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B14" s="2">
         <v>11</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="2">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="2">
         <v>1.06E-3</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E14" s="2">
         <v>0.591229</v>
       </c>
-      <c r="F14" s="14">
+      <c r="F14" s="7">
         <v>67.768906000000001</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="8">
         <v>919.22993199999996</v>
       </c>
-      <c r="I14" s="16">
+      <c r="I14" s="2">
         <v>11</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="2">
         <v>1.22E-4</v>
       </c>
-      <c r="K14" s="13">
+      <c r="K14" s="2">
         <v>2.1229999999999999E-3</v>
       </c>
-      <c r="L14" s="13">
+      <c r="L14" s="2">
         <v>0.57476099999999997</v>
       </c>
-      <c r="M14" s="13">
+      <c r="M14" s="2">
         <v>68.609347</v>
       </c>
-      <c r="N14" s="13">
+      <c r="N14" s="2">
         <v>904.03103299999998</v>
       </c>
+      <c r="P14" s="2">
+        <v>5</v>
+      </c>
+      <c r="Q14" s="2">
+        <f t="shared" si="0"/>
+        <v>1.7077353424610371E-5</v>
+      </c>
+      <c r="R14" s="2">
+        <f t="shared" si="1"/>
+        <v>1.8274214211714212E-5</v>
+      </c>
+      <c r="S14" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7327826963417237E-5</v>
+      </c>
+      <c r="T14" s="15">
+        <f t="shared" si="3"/>
+        <v>1.6888314874425987E-5</v>
+      </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="16">
+    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B15" s="2">
         <v>12</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="2">
         <v>8.6000000000000003E-5</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="2">
         <v>1.011E-3</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="2">
         <v>0.56484900000000005</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="7">
         <v>71.301658000000003</v>
       </c>
-      <c r="G15" s="15">
+      <c r="G15" s="8">
         <v>857.31556999999998</v>
       </c>
-      <c r="I15" s="16">
+      <c r="I15" s="2">
         <v>12</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="2">
         <v>1.1E-4</v>
       </c>
-      <c r="K15" s="13">
+      <c r="K15" s="2">
         <v>2.1359999999999999E-3</v>
       </c>
-      <c r="L15" s="13">
+      <c r="L15" s="2">
         <v>0.57728599999999997</v>
       </c>
-      <c r="M15" s="13">
+      <c r="M15" s="2">
         <v>69.900491000000002</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="2">
         <v>904.52477399999998</v>
       </c>
+      <c r="P15" s="2">
+        <v>6</v>
+      </c>
+      <c r="Q15" s="2">
+        <f>$Q$3*FACT(P15)</f>
+        <v>1.0246412054766223E-4</v>
+      </c>
+      <c r="R15" s="2">
+        <f>$Q$4*FACT(P15)</f>
+        <v>1.0964528527028526E-4</v>
+      </c>
+      <c r="S15" s="2">
+        <f>$Q$5*FACT(P15)</f>
+        <v>1.0396696178050344E-4</v>
+      </c>
+      <c r="T15" s="15">
+        <f>$Q$6*FACT(P15)</f>
+        <v>1.0132988924655593E-4</v>
+      </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="16">
+    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
         <v>13</v>
       </c>
-      <c r="C16" s="13">
+      <c r="C16" s="2">
         <v>3.8000000000000002E-5</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="2">
         <v>1.018E-3</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="2">
         <v>0.60061200000000003</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="7">
         <v>70.395849999999996</v>
       </c>
-      <c r="G16" s="15">
+      <c r="G16" s="8">
         <v>897.37232200000005</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="2">
         <v>13</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="2">
         <v>1.08E-4</v>
       </c>
-      <c r="K16" s="13">
+      <c r="K16" s="2">
         <v>2.1120000000000002E-3</v>
       </c>
-      <c r="L16" s="13">
+      <c r="L16" s="2">
         <v>0.57594299999999998</v>
       </c>
-      <c r="M16" s="13">
+      <c r="M16" s="2">
         <v>69.574625999999995</v>
       </c>
-      <c r="N16" s="13">
+      <c r="N16" s="2">
         <v>902.913006</v>
       </c>
+      <c r="P16" s="2">
+        <v>7</v>
+      </c>
+      <c r="Q16" s="2">
+        <f t="shared" ref="Q16:Q24" si="4">$Q$3*FACT(P16)</f>
+        <v>7.1724884383363564E-4</v>
+      </c>
+      <c r="R16" s="2">
+        <f t="shared" ref="R16:R24" si="5">$Q$4*FACT(P16)</f>
+        <v>7.6751699689199678E-4</v>
+      </c>
+      <c r="S16" s="2">
+        <f t="shared" ref="S16:S24" si="6">$Q$5*FACT(P16)</f>
+        <v>7.2776873246352403E-4</v>
+      </c>
+      <c r="T16" s="15">
+        <f t="shared" ref="T16:T24" si="7">$Q$6*FACT(P16)</f>
+        <v>7.0930922472589152E-4</v>
+      </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="16">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B17" s="2">
         <v>14</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="2">
         <v>3.6000000000000001E-5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="2">
         <v>1.067E-3</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="2">
         <v>0.59314500000000003</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="7">
         <v>67.694800000000001</v>
       </c>
-      <c r="G17" s="15">
+      <c r="G17" s="8">
         <v>881.25936200000001</v>
       </c>
-      <c r="I17" s="16">
+      <c r="I17" s="2">
         <v>14</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="2">
         <v>1.0900000000000001E-4</v>
       </c>
-      <c r="K17" s="13">
+      <c r="K17" s="2">
         <v>2.055E-3</v>
       </c>
-      <c r="L17" s="13">
+      <c r="L17" s="2">
         <v>0.58266200000000001</v>
       </c>
-      <c r="M17" s="13">
+      <c r="M17" s="2">
         <v>69.567784000000003</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="2">
         <v>903.04707800000006</v>
       </c>
+      <c r="P17" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q17" s="2">
+        <f t="shared" si="4"/>
+        <v>5.7379907506690852E-3</v>
+      </c>
+      <c r="R17" s="2">
+        <f t="shared" si="5"/>
+        <v>6.1401359751359743E-3</v>
+      </c>
+      <c r="S17" s="2">
+        <f t="shared" si="6"/>
+        <v>5.8221498597081922E-3</v>
+      </c>
+      <c r="T17" s="15">
+        <f t="shared" si="7"/>
+        <v>5.6744737978071322E-3</v>
+      </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="16">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B18" s="2">
         <v>15</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="2">
         <v>3.6999999999999998E-5</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18" s="2">
         <v>1.023E-3</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E18" s="2">
         <v>0.59454600000000002</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="7">
         <v>67.169049999999999</v>
       </c>
-      <c r="G18" s="15">
+      <c r="G18" s="8">
         <v>883.04720399999997</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="2">
         <v>15</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="2">
         <v>1.13E-4</v>
       </c>
-      <c r="K18" s="13">
+      <c r="K18" s="2">
         <v>1.815E-3</v>
       </c>
-      <c r="L18" s="13">
+      <c r="L18" s="2">
         <v>0.57867299999999999</v>
       </c>
-      <c r="M18" s="13">
+      <c r="M18" s="2">
         <v>69.605817999999999</v>
       </c>
-      <c r="N18" s="13">
+      <c r="N18" s="2">
         <v>902.321325</v>
       </c>
+      <c r="P18" s="2">
+        <v>9</v>
+      </c>
+      <c r="Q18" s="2">
+        <f t="shared" si="4"/>
+        <v>5.1641916756021762E-2</v>
+      </c>
+      <c r="R18" s="2">
+        <f t="shared" si="5"/>
+        <v>5.5261223776223771E-2</v>
+      </c>
+      <c r="S18" s="2">
+        <f t="shared" si="6"/>
+        <v>5.239934873737373E-2</v>
+      </c>
+      <c r="T18" s="15">
+        <f t="shared" si="7"/>
+        <v>5.107026418026419E-2</v>
+      </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="3">
         <f>AVERAGE(C4:C18)</f>
         <v>4.8266666666666677E-5</v>
       </c>
-      <c r="D19" s="8">
-        <f t="shared" ref="D19:F19" si="0">AVERAGE(D4:D18)</f>
+      <c r="D19" s="3">
+        <f t="shared" ref="D19:F19" si="8">AVERAGE(D4:D18)</f>
         <v>1.0730000000000002E-3</v>
       </c>
-      <c r="E19" s="8">
-        <f t="shared" si="0"/>
+      <c r="E19" s="3">
+        <f t="shared" si="8"/>
         <v>0.58585586666666656</v>
       </c>
-      <c r="F19" s="8">
-        <f t="shared" si="0"/>
+      <c r="F19" s="3">
+        <f t="shared" si="8"/>
         <v>69.729294333333343</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="3">
         <f>AVERAGE(G4:G18)</f>
         <v>886.17529153333339</v>
       </c>
-      <c r="I19" s="7" t="s">
+      <c r="I19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="3">
         <f>AVERAGE(J4:J18)</f>
         <v>9.0533333333333343E-5</v>
       </c>
-      <c r="K19" s="8">
-        <f t="shared" ref="K19" si="1">AVERAGE(K4:K18)</f>
+      <c r="K19" s="3">
+        <f t="shared" ref="K19" si="9">AVERAGE(K4:K18)</f>
         <v>2.4733999999999997E-3</v>
       </c>
-      <c r="L19" s="8">
-        <f t="shared" ref="L19" si="2">AVERAGE(L4:L18)</f>
+      <c r="L19" s="3">
+        <f t="shared" ref="L19" si="10">AVERAGE(L4:L18)</f>
         <v>0.58034513333333337</v>
       </c>
-      <c r="M19" s="8">
-        <f t="shared" ref="M19" si="3">AVERAGE(M4:M18)</f>
+      <c r="M19" s="3">
+        <f t="shared" ref="M19" si="11">AVERAGE(M4:M18)</f>
         <v>68.218839133333319</v>
       </c>
-      <c r="N19" s="8">
-        <f t="shared" ref="N19" si="4">AVERAGE(N4:N18)</f>
+      <c r="N19" s="3">
+        <f t="shared" ref="N19" si="12">AVERAGE(N4:N18)</f>
         <v>899.17282433333321</v>
       </c>
+      <c r="P19" s="2">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="2">
+        <f t="shared" si="4"/>
+        <v>0.51641916756021766</v>
+      </c>
+      <c r="R19" s="2">
+        <f t="shared" si="5"/>
+        <v>0.55261223776223767</v>
+      </c>
+      <c r="S19" s="2">
+        <f t="shared" si="6"/>
+        <v>0.5239934873737373</v>
+      </c>
+      <c r="T19" s="15">
+        <f t="shared" si="7"/>
+        <v>0.51070264180264191</v>
+      </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="10" t="s">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="P20" s="2">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="2">
+        <f t="shared" si="4"/>
+        <v>5.6806108431623938</v>
+      </c>
+      <c r="R20" s="2">
+        <f t="shared" si="5"/>
+        <v>6.0787346153846151</v>
+      </c>
+      <c r="S20" s="2">
+        <f t="shared" si="6"/>
+        <v>5.7639283611111098</v>
+      </c>
+      <c r="T20" s="15">
+        <f t="shared" si="7"/>
+        <v>5.6177290598290606</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="P21" s="2">
+        <v>12</v>
+      </c>
+      <c r="Q21" s="2">
+        <f t="shared" si="4"/>
+        <v>68.167330117948723</v>
+      </c>
+      <c r="R21" s="2">
+        <f t="shared" si="5"/>
+        <v>72.944815384615382</v>
+      </c>
+      <c r="S21" s="2">
+        <f t="shared" si="6"/>
+        <v>69.167140333333322</v>
+      </c>
+      <c r="T21" s="15">
+        <f t="shared" si="7"/>
+        <v>67.41274871794873</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="I22" s="10" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="I22" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="P22" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q22" s="2">
+        <f t="shared" si="4"/>
+        <v>886.17529153333339</v>
+      </c>
+      <c r="R22" s="2">
+        <f t="shared" si="5"/>
+        <v>948.28259999999989</v>
+      </c>
+      <c r="S22" s="2">
+        <f t="shared" si="6"/>
+        <v>899.17282433333321</v>
+      </c>
+      <c r="T22" s="15">
+        <f t="shared" si="7"/>
+        <v>876.36573333333342</v>
+      </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="6" t="s">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="3">
         <v>5</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="3">
         <v>7</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="3">
         <v>10</v>
       </c>
-      <c r="F23" s="12">
+      <c r="F23" s="6">
         <v>12</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="5">
         <v>13</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I23" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J23" s="6">
+      <c r="J23" s="3">
         <v>5</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="3">
         <v>7</v>
       </c>
-      <c r="L23" s="6">
+      <c r="L23" s="3">
         <v>10</v>
       </c>
-      <c r="M23" s="12">
+      <c r="M23" s="6">
         <v>12</v>
       </c>
-      <c r="N23" s="9">
+      <c r="N23" s="5">
         <v>13</v>
       </c>
+      <c r="P23" s="2">
+        <v>14</v>
+      </c>
+      <c r="Q23" s="2">
+        <f t="shared" si="4"/>
+        <v>12406.454081466669</v>
+      </c>
+      <c r="R23" s="2">
+        <f t="shared" si="5"/>
+        <v>13275.956399999999</v>
+      </c>
+      <c r="S23" s="2">
+        <f t="shared" si="6"/>
+        <v>12588.419540666664</v>
+      </c>
+      <c r="T23" s="15">
+        <f t="shared" si="7"/>
+        <v>12269.120266666669</v>
+      </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="16">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B24" s="2">
         <v>1</v>
       </c>
-      <c r="C24" s="13">
+      <c r="C24" s="2">
         <v>0</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E24" s="13">
+      <c r="E24" s="2">
         <v>0.58099999999999996</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="2">
         <v>77.986999999999995</v>
       </c>
-      <c r="G24" s="13">
+      <c r="G24" s="2">
         <v>859.81700000000001</v>
       </c>
-      <c r="I24" s="16">
+      <c r="I24" s="2">
         <v>1</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="2">
         <v>0</v>
       </c>
-      <c r="K24" s="13">
+      <c r="K24" s="2">
         <v>0</v>
       </c>
-      <c r="L24" s="13">
+      <c r="L24" s="2">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N24" s="2">
+        <v>955.96799999999996</v>
+      </c>
+      <c r="P24" s="2">
+        <v>15</v>
+      </c>
+      <c r="Q24" s="2">
+        <f t="shared" si="4"/>
+        <v>186096.81122200002</v>
+      </c>
+      <c r="R24" s="2">
+        <f t="shared" si="5"/>
+        <v>199139.34599999999</v>
+      </c>
+      <c r="S24" s="2">
+        <f t="shared" si="6"/>
+        <v>188826.29310999997</v>
+      </c>
+      <c r="T24" s="15">
+        <f t="shared" si="7"/>
+        <v>184036.80400000003</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B25" s="2">
+        <v>2</v>
+      </c>
+      <c r="C25" s="2">
         <v>0</v>
       </c>
-      <c r="M24" s="13">
+      <c r="D25" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.58299999999999996</v>
+      </c>
+      <c r="F25" s="2">
+        <v>77.272999999999996</v>
+      </c>
+      <c r="G25" s="2">
+        <v>857.47</v>
+      </c>
+      <c r="I25" s="2">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2">
         <v>0</v>
       </c>
-      <c r="N24" s="13">
+      <c r="K25" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="L25" s="2">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="M25" s="2">
+        <v>68.058999999999997</v>
+      </c>
+      <c r="N25" s="2">
+        <v>910.86</v>
+      </c>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B26" s="2">
+        <v>3</v>
+      </c>
+      <c r="C26" s="2">
         <v>0</v>
       </c>
+      <c r="D26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="F26" s="2">
+        <v>76.853999999999999</v>
+      </c>
+      <c r="G26" s="2">
+        <v>854.726</v>
+      </c>
+      <c r="I26" s="2">
+        <v>3</v>
+      </c>
+      <c r="J26" s="2">
+        <v>0</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0.51500000000000001</v>
+      </c>
+      <c r="M26" s="2">
+        <v>67.334000000000003</v>
+      </c>
+      <c r="N26" s="2">
+        <v>869.18700000000001</v>
+      </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="16">
-        <v>2</v>
-      </c>
-      <c r="C25" s="13">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B27" s="2">
+        <v>4</v>
+      </c>
+      <c r="C27" s="2">
         <v>0</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D27" s="2">
+        <v>0</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="F27" s="2">
+        <v>79.584999999999994</v>
+      </c>
+      <c r="G27" s="2">
+        <v>859.99599999999998</v>
+      </c>
+      <c r="I27" s="2">
+        <v>4</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0</v>
+      </c>
+      <c r="K27" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E25" s="13">
-        <v>0.58299999999999996</v>
-      </c>
-      <c r="F25" s="13">
-        <v>77.272999999999996</v>
-      </c>
-      <c r="G25" s="13">
-        <v>857.47</v>
-      </c>
-      <c r="I25" s="16">
-        <v>2</v>
-      </c>
-      <c r="J25" s="13">
+      <c r="L27" s="2">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="M27" s="2">
+        <v>68.358000000000004</v>
+      </c>
+      <c r="N27" s="2">
+        <v>873.19200000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B28" s="2">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2">
         <v>0</v>
       </c>
-      <c r="K25" s="13">
+      <c r="D28" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="F28" s="2">
+        <v>77.947999999999993</v>
+      </c>
+      <c r="G28" s="2">
+        <v>919.50800000000004</v>
+      </c>
+      <c r="I28" s="2">
+        <v>5</v>
+      </c>
+      <c r="J28" s="2">
         <v>0</v>
       </c>
-      <c r="L25" s="13">
+      <c r="K28" s="2">
         <v>0</v>
       </c>
-      <c r="M25" s="13">
+      <c r="L28" s="2">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="M28" s="2">
+        <v>70.256</v>
+      </c>
+      <c r="N28" s="2">
+        <v>872.476</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B29" s="2">
+        <v>6</v>
+      </c>
+      <c r="C29" s="2">
         <v>0</v>
       </c>
-      <c r="N25" s="13">
+      <c r="D29" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="F29" s="2">
+        <v>73.369</v>
+      </c>
+      <c r="G29" s="2">
+        <v>949.37</v>
+      </c>
+      <c r="I29" s="2">
+        <v>6</v>
+      </c>
+      <c r="J29" s="2">
         <v>0</v>
       </c>
+      <c r="K29" s="2">
+        <v>0</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="M29" s="2">
+        <v>67.236000000000004</v>
+      </c>
+      <c r="N29" s="2">
+        <v>866.44799999999998</v>
+      </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="16">
-        <v>3</v>
-      </c>
-      <c r="C26" s="13">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B30" s="2">
+        <v>7</v>
+      </c>
+      <c r="C30" s="2">
         <v>0</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D30" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E26" s="13">
-        <v>0.56699999999999995</v>
-      </c>
-      <c r="F26" s="13">
-        <v>76.853999999999999</v>
-      </c>
-      <c r="G26" s="13">
-        <v>854.726</v>
-      </c>
-      <c r="I26" s="16">
-        <v>3</v>
-      </c>
-      <c r="J26" s="13">
+      <c r="E30" s="2">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="F30" s="2">
+        <v>67.111999999999995</v>
+      </c>
+      <c r="G30" s="2">
+        <v>993.71299999999997</v>
+      </c>
+      <c r="I30" s="2">
+        <v>7</v>
+      </c>
+      <c r="J30" s="2">
         <v>0</v>
       </c>
-      <c r="K26" s="13">
+      <c r="K30" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="M30" s="2">
+        <v>68.066999999999993</v>
+      </c>
+      <c r="N30" s="2">
+        <v>873.08900000000006</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B31" s="2">
+        <v>8</v>
+      </c>
+      <c r="C31" s="2">
         <v>0</v>
       </c>
-      <c r="L26" s="13">
+      <c r="D31" s="2">
         <v>0</v>
       </c>
-      <c r="M26" s="13">
+      <c r="E31" s="2">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F31" s="2">
+        <v>66.84</v>
+      </c>
+      <c r="G31" s="2">
+        <v>1039.277</v>
+      </c>
+      <c r="I31" s="2">
+        <v>8</v>
+      </c>
+      <c r="J31" s="2">
         <v>0</v>
       </c>
-      <c r="N26" s="13">
+      <c r="K31" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="M31" s="2">
+        <v>68.799000000000007</v>
+      </c>
+      <c r="N31" s="2">
+        <v>873.38099999999997</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20" x14ac:dyDescent="0.2">
+      <c r="B32" s="2">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="16">
-        <v>4</v>
-      </c>
-      <c r="C27" s="13">
+      <c r="D32" s="2">
+        <v>2E-3</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="F32" s="2">
+        <v>67.522000000000006</v>
+      </c>
+      <c r="G32" s="2">
+        <v>969.779</v>
+      </c>
+      <c r="I32" s="2">
+        <v>9</v>
+      </c>
+      <c r="J32" s="2">
         <v>0</v>
       </c>
-      <c r="D27" s="13">
-        <v>0</v>
-      </c>
-      <c r="E27" s="13">
-        <v>0.58199999999999996</v>
-      </c>
-      <c r="F27" s="13">
-        <v>79.584999999999994</v>
-      </c>
-      <c r="G27" s="13">
-        <v>859.99599999999998</v>
-      </c>
-      <c r="I27" s="16">
-        <v>4</v>
-      </c>
-      <c r="J27" s="13">
-        <v>0</v>
-      </c>
-      <c r="K27" s="13">
-        <v>0</v>
-      </c>
-      <c r="L27" s="13">
-        <v>0</v>
-      </c>
-      <c r="M27" s="13">
-        <v>0</v>
-      </c>
-      <c r="N27" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="16">
-        <v>5</v>
-      </c>
-      <c r="C28" s="13">
-        <v>0</v>
-      </c>
-      <c r="D28" s="13">
+      <c r="K32" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E28" s="13">
-        <v>0.56299999999999994</v>
-      </c>
-      <c r="F28" s="13">
-        <v>77.947999999999993</v>
-      </c>
-      <c r="G28" s="13">
-        <v>919.50800000000004</v>
-      </c>
-      <c r="I28" s="16">
-        <v>5</v>
-      </c>
-      <c r="J28" s="13">
-        <v>0</v>
-      </c>
-      <c r="K28" s="13">
-        <v>0</v>
-      </c>
-      <c r="L28" s="13">
-        <v>0</v>
-      </c>
-      <c r="M28" s="13">
-        <v>0</v>
-      </c>
-      <c r="N28" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="16">
-        <v>6</v>
-      </c>
-      <c r="C29" s="13">
-        <v>0</v>
-      </c>
-      <c r="D29" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="E29" s="13">
-        <v>0.64100000000000001</v>
-      </c>
-      <c r="F29" s="13">
-        <v>73.369</v>
-      </c>
-      <c r="G29" s="13">
-        <v>949.37</v>
-      </c>
-      <c r="I29" s="16">
-        <v>6</v>
-      </c>
-      <c r="J29" s="13">
-        <v>0</v>
-      </c>
-      <c r="K29" s="13">
-        <v>0</v>
-      </c>
-      <c r="L29" s="13">
-        <v>0</v>
-      </c>
-      <c r="M29" s="13">
-        <v>0</v>
-      </c>
-      <c r="N29" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="16">
-        <v>7</v>
-      </c>
-      <c r="C30" s="13">
-        <v>0</v>
-      </c>
-      <c r="D30" s="13">
-        <v>1E-3</v>
-      </c>
-      <c r="E30" s="13">
-        <v>0.57899999999999996</v>
-      </c>
-      <c r="F30" s="13">
-        <v>67.111999999999995</v>
-      </c>
-      <c r="G30" s="13">
-        <v>993.71299999999997</v>
-      </c>
-      <c r="I30" s="16">
-        <v>7</v>
-      </c>
-      <c r="J30" s="13">
-        <v>0</v>
-      </c>
-      <c r="K30" s="13">
-        <v>0</v>
-      </c>
-      <c r="L30" s="13">
-        <v>0</v>
-      </c>
-      <c r="M30" s="13">
-        <v>0</v>
-      </c>
-      <c r="N30" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="16">
-        <v>8</v>
-      </c>
-      <c r="C31" s="13">
-        <v>0</v>
-      </c>
-      <c r="D31" s="13">
-        <v>0</v>
-      </c>
-      <c r="E31" s="13">
-        <v>0.67300000000000004</v>
-      </c>
-      <c r="F31" s="13">
-        <v>66.84</v>
-      </c>
-      <c r="G31" s="13">
-        <v>1039.277</v>
-      </c>
-      <c r="I31" s="16">
-        <v>8</v>
-      </c>
-      <c r="J31" s="13">
-        <v>0</v>
-      </c>
-      <c r="K31" s="13">
-        <v>0</v>
-      </c>
-      <c r="L31" s="13">
-        <v>0</v>
-      </c>
-      <c r="M31" s="13">
-        <v>0</v>
-      </c>
-      <c r="N31" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="16">
-        <v>9</v>
-      </c>
-      <c r="C32" s="13">
-        <v>0</v>
-      </c>
-      <c r="D32" s="13">
-        <v>2E-3</v>
-      </c>
-      <c r="E32" s="13">
-        <v>0.67300000000000004</v>
-      </c>
-      <c r="F32" s="13">
-        <v>67.522000000000006</v>
-      </c>
-      <c r="G32" s="13">
-        <v>969.779</v>
-      </c>
-      <c r="I32" s="16">
-        <v>9</v>
-      </c>
-      <c r="J32" s="13">
-        <v>0</v>
-      </c>
-      <c r="K32" s="13">
-        <v>0</v>
-      </c>
-      <c r="L32" s="13">
-        <v>0</v>
-      </c>
-      <c r="M32" s="13">
-        <v>0</v>
-      </c>
-      <c r="N32" s="13">
-        <v>0</v>
+      <c r="L32" s="2">
+        <v>0.52100000000000002</v>
+      </c>
+      <c r="M32" s="2">
+        <v>67.242999999999995</v>
+      </c>
+      <c r="N32" s="2">
+        <v>863.58799999999997</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B33" s="16">
+      <c r="B33" s="2">
         <v>10</v>
       </c>
-      <c r="C33" s="13">
+      <c r="C33" s="2">
         <v>0</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33" s="2">
         <v>0</v>
       </c>
-      <c r="E33" s="13">
+      <c r="E33" s="2">
         <v>0.56999999999999995</v>
       </c>
-      <c r="F33" s="13">
+      <c r="F33" s="2">
         <v>67.322000000000003</v>
       </c>
-      <c r="G33" s="13">
+      <c r="G33" s="2">
         <v>1426.3309999999999</v>
       </c>
-      <c r="I33" s="16">
+      <c r="I33" s="2">
         <v>10</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="2">
         <v>0</v>
       </c>
-      <c r="K33" s="13">
-        <v>0</v>
-      </c>
-      <c r="L33" s="13">
-        <v>0</v>
-      </c>
-      <c r="M33" s="13">
-        <v>0</v>
-      </c>
-      <c r="N33" s="13">
-        <v>0</v>
+      <c r="K33" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0.52200000000000002</v>
+      </c>
+      <c r="M33" s="2">
+        <v>67.099999999999994</v>
+      </c>
+      <c r="N33" s="2">
+        <v>859.995</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="16">
+      <c r="B34" s="2">
         <v>11</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="2">
         <v>0</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="2">
         <v>2E-3</v>
       </c>
-      <c r="E34" s="13">
+      <c r="E34" s="2">
         <v>0.57099999999999995</v>
       </c>
-      <c r="F34" s="13">
+      <c r="F34" s="2">
         <v>68.34</v>
       </c>
-      <c r="G34" s="13">
+      <c r="G34" s="2">
         <v>880.62599999999998</v>
       </c>
-      <c r="I34" s="16">
+      <c r="I34" s="2">
         <v>11</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="2">
         <v>0</v>
       </c>
-      <c r="K34" s="13">
-        <v>0</v>
-      </c>
-      <c r="L34" s="13">
-        <v>0</v>
-      </c>
-      <c r="M34" s="13">
-        <v>0</v>
-      </c>
-      <c r="N34" s="13">
-        <v>0</v>
+      <c r="K34" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="M34" s="2">
+        <v>67.191999999999993</v>
+      </c>
+      <c r="N34" s="2">
+        <v>891.13099999999997</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="16">
+      <c r="B35" s="2">
         <v>12</v>
       </c>
-      <c r="C35" s="13">
+      <c r="C35" s="2">
         <v>0</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E35" s="13">
+      <c r="E35" s="2">
         <v>0.65500000000000003</v>
       </c>
-      <c r="F35" s="13">
+      <c r="F35" s="2">
         <v>66.381</v>
       </c>
-      <c r="G35" s="13">
+      <c r="G35" s="2">
         <v>909.29200000000003</v>
       </c>
-      <c r="I35" s="16">
+      <c r="I35" s="2">
         <v>12</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="2">
         <v>0</v>
       </c>
-      <c r="K35" s="13">
-        <v>0</v>
-      </c>
-      <c r="L35" s="13">
-        <v>0</v>
-      </c>
-      <c r="M35" s="13">
-        <v>0</v>
-      </c>
-      <c r="N35" s="13">
-        <v>0</v>
+      <c r="K35" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="M35" s="2">
+        <v>6.2510000000000003</v>
+      </c>
+      <c r="N35" s="2">
+        <v>863.69100000000003</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="16">
+      <c r="B36" s="2">
         <v>13</v>
       </c>
-      <c r="C36" s="13">
+      <c r="C36" s="2">
         <v>0</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E36" s="13">
+      <c r="E36" s="2">
         <v>0.59399999999999997</v>
       </c>
-      <c r="F36" s="13">
+      <c r="F36" s="2">
         <v>65.631</v>
       </c>
-      <c r="G36" s="13">
+      <c r="G36" s="2">
         <v>902.40099999999995</v>
       </c>
-      <c r="I36" s="16">
+      <c r="I36" s="2">
         <v>13</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="2">
         <v>0</v>
       </c>
-      <c r="K36" s="13">
-        <v>0</v>
-      </c>
-      <c r="L36" s="13">
-        <v>0</v>
-      </c>
-      <c r="M36" s="13">
-        <v>0</v>
-      </c>
-      <c r="N36" s="13">
-        <v>0</v>
+      <c r="K36" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L36" s="2">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="M36" s="2">
+        <v>67.08</v>
+      </c>
+      <c r="N36" s="2">
+        <v>856.92499999999995</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="16">
+      <c r="B37" s="2">
         <v>14</v>
       </c>
-      <c r="C37" s="13">
+      <c r="C37" s="2">
         <v>0</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="2">
         <v>2E-3</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E37" s="2">
         <v>0.54700000000000004</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F37" s="2">
         <v>65.620999999999995</v>
       </c>
-      <c r="G37" s="13">
+      <c r="G37" s="2">
         <v>901.55899999999997</v>
       </c>
-      <c r="I37" s="16">
+      <c r="I37" s="2">
         <v>14</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="2">
         <v>0</v>
       </c>
-      <c r="K37" s="13">
-        <v>0</v>
-      </c>
-      <c r="L37" s="13">
-        <v>0</v>
-      </c>
-      <c r="M37" s="13">
-        <v>0</v>
-      </c>
-      <c r="N37" s="13">
-        <v>0</v>
+      <c r="K37" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="M37" s="2">
+        <v>67.192999999999998</v>
+      </c>
+      <c r="N37" s="2">
+        <v>857.99300000000005</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="16">
+      <c r="B38" s="2">
         <v>15</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="2">
         <v>0</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="2">
         <v>1E-3</v>
       </c>
-      <c r="E38" s="13">
+      <c r="E38" s="2">
         <v>0.60699999999999998</v>
       </c>
-      <c r="F38" s="13">
+      <c r="F38" s="2">
         <v>65.831999999999994</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G38" s="2">
         <v>900.37400000000002</v>
       </c>
-      <c r="I38" s="16">
+      <c r="I38" s="2">
         <v>15</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="2">
         <v>0</v>
       </c>
-      <c r="K38" s="13">
-        <v>0</v>
-      </c>
-      <c r="L38" s="13">
-        <v>0</v>
-      </c>
-      <c r="M38" s="13">
-        <v>0</v>
-      </c>
-      <c r="N38" s="13">
-        <v>0</v>
+      <c r="K38" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0.52600000000000002</v>
+      </c>
+      <c r="M38" s="2">
+        <v>67.396000000000001</v>
+      </c>
+      <c r="N38" s="2">
+        <v>857.56200000000001</v>
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="3">
         <f>AVERAGE(C24:C38)</f>
         <v>0</v>
       </c>
-      <c r="D39" s="8">
-        <f t="shared" ref="D39" si="5">AVERAGE(D24:D38)</f>
+      <c r="D39" s="3">
+        <f t="shared" ref="D39" si="13">AVERAGE(D24:D38)</f>
         <v>1E-3</v>
       </c>
-      <c r="E39" s="8">
-        <f t="shared" ref="E39" si="6">AVERAGE(E24:E38)</f>
+      <c r="E39" s="3">
+        <f t="shared" ref="E39" si="14">AVERAGE(E24:E38)</f>
         <v>0.59906666666666664</v>
       </c>
-      <c r="F39" s="8">
-        <f t="shared" ref="F39" si="7">AVERAGE(F24:F38)</f>
+      <c r="F39" s="3">
+        <f t="shared" ref="F39" si="15">AVERAGE(F24:F38)</f>
         <v>70.907799999999995</v>
       </c>
-      <c r="G39" s="8">
-        <f t="shared" ref="G39" si="8">AVERAGE(G24:G38)</f>
+      <c r="G39" s="3">
+        <f t="shared" ref="G39" si="16">AVERAGE(G24:G38)</f>
         <v>948.28259999999989</v>
       </c>
-      <c r="I39" s="7" t="s">
+      <c r="I39" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="J39" s="8">
+      <c r="J39" s="3">
         <f>AVERAGE(J24:J38)</f>
         <v>0</v>
       </c>
-      <c r="K39" s="8">
-        <f t="shared" ref="K39" si="9">AVERAGE(K24:K38)</f>
-        <v>0</v>
-      </c>
-      <c r="L39" s="8">
-        <f t="shared" ref="L39" si="10">AVERAGE(L24:L38)</f>
-        <v>0</v>
-      </c>
-      <c r="M39" s="8">
-        <f t="shared" ref="M39" si="11">AVERAGE(M24:M38)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="8">
-        <f t="shared" ref="N39" si="12">AVERAGE(N24:N38)</f>
-        <v>0</v>
+      <c r="K39" s="3">
+        <f t="shared" ref="K39" si="17">AVERAGE(K24:K38)</f>
+        <v>8.6666666666666695E-4</v>
+      </c>
+      <c r="L39" s="3">
+        <f t="shared" ref="L39" si="18">AVERAGE(L24:L38)</f>
+        <v>0.52839999999999998</v>
+      </c>
+      <c r="M39" s="3">
+        <f t="shared" ref="M39" si="19">AVERAGE(M24:M38)</f>
+        <v>63.397428571428577</v>
+      </c>
+      <c r="N39" s="3">
+        <f t="shared" ref="N39" si="20">AVERAGE(N24:N38)</f>
+        <v>876.36573333333342</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P8:T8"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B22:G22"/>

</xml_diff>